<commit_message>
Added Features: - Great Sword motion values - New CSV format
</commit_message>
<xml_diff>
--- a/files/weapons/dualblades_mv.xlsx
+++ b/files/weapons/dualblades_mv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evenn\PycharmProjects\MHWIceborneCalculator\files\weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07896AFF-47ED-4D1D-ABDD-C3B8335CD308}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6885B957-B60D-499F-A734-3276C9023BFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{9EE5A8B1-BBE0-4EA1-88E1-CCE30DD6F00F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9EE5A8B1-BBE0-4EA1-88E1-CCE30DD6F00F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Attack 1</t>
   </si>
@@ -72,27 +72,9 @@
     <t>Double Slash Return</t>
   </si>
   <si>
-    <t>Rotation Slash</t>
-  </si>
-  <si>
-    <t>Draw Slash</t>
-  </si>
-  <si>
     <t>Rising Slash</t>
   </si>
   <si>
-    <t>Demonized Revers Slash</t>
-  </si>
-  <si>
-    <t>Demonized Double Slash</t>
-  </si>
-  <si>
-    <t>Demonized 6-Step Slash</t>
-  </si>
-  <si>
-    <t>Demon Dance</t>
-  </si>
-  <si>
     <t>Attack 12</t>
   </si>
   <si>
@@ -108,25 +90,67 @@
     <t>Attack 16</t>
   </si>
   <si>
-    <t>Demon Rush Slash</t>
-  </si>
-  <si>
-    <t>Demon Continuous Slash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left Rotation Slash </t>
-  </si>
-  <si>
-    <t>Right Rotation Slash</t>
-  </si>
-  <si>
-    <t>Rotating Demon Dance Finish</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Aerial Roration Demon Dance (10 Hits)</t>
+    <t>Circle Slash</t>
+  </si>
+  <si>
+    <t>Lunging Strike</t>
+  </si>
+  <si>
+    <t>Left Round Slash</t>
+  </si>
+  <si>
+    <t>Right Round Slash</t>
+  </si>
+  <si>
+    <t>Turn Slash</t>
+  </si>
+  <si>
+    <t>Sliding Slash</t>
+  </si>
+  <si>
+    <t>Demon Fangs</t>
+  </si>
+  <si>
+    <t>Twofold Demon Slash</t>
+  </si>
+  <si>
+    <t>Sixfold Demon Slash</t>
+  </si>
+  <si>
+    <t>Demon Flurry Rush</t>
+  </si>
+  <si>
+    <t>Right Fade Slash</t>
+  </si>
+  <si>
+    <t>Left Fade Slash</t>
+  </si>
+  <si>
+    <t>Right Double Round Slash</t>
+  </si>
+  <si>
+    <t>Left Double Round Slash</t>
+  </si>
+  <si>
+    <t>Blade Dance</t>
+  </si>
+  <si>
+    <t>Demon Flurry</t>
+  </si>
+  <si>
+    <t>Jumping Double Slash</t>
+  </si>
+  <si>
+    <t>Heavenly Blade Dance</t>
+  </si>
+  <si>
+    <t>Midair Spinning Blade Dance</t>
+  </si>
+  <si>
+    <t>Spinning Blade Dance Finisher</t>
   </si>
 </sst>
 </file>
@@ -484,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A44345-711C-400E-94FC-0F3218E45614}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +521,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -533,19 +557,19 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -553,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -606,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -656,13 +680,13 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>11</v>
@@ -709,13 +733,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -762,16 +786,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>15</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -815,16 +839,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -868,13 +892,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -921,25 +945,25 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -974,78 +998,78 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1080,28 +1104,28 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1133,25 +1157,25 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
         <v>16</v>
       </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1186,25 +1210,25 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
         <v>8</v>
       </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1239,10 +1263,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1292,59 +1316,484 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>11</v>
+      </c>
+      <c r="K19">
+        <v>11</v>
+      </c>
+      <c r="L19">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>12</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>12</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>17</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <v>12</v>
+      </c>
+      <c r="J22">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="K22">
         <v>21</v>
       </c>
-      <c r="D16">
-        <v>11</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>